<commit_message>
more transfer report stuff
</commit_message>
<xml_diff>
--- a/1810_FSE_for-serious-this-time.xlsx
+++ b/1810_FSE_for-serious-this-time.xlsx
@@ -19,6 +19,7 @@
     <sheet name="4000K-paper1 figure dump" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4489,6 +4490,9 @@
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.18871317840493429</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18590621037263885</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.15398737068883597</c:v>
@@ -15436,8 +15440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34:P38"/>
+    <sheetView tabSelected="1" topLeftCell="J7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16808,7 +16812,9 @@
       <c r="C34" s="8">
         <v>5.2990469899999999</v>
       </c>
-      <c r="D34" s="8"/>
+      <c r="D34" s="8">
+        <v>5.3790564500000002</v>
+      </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
@@ -16820,20 +16826,23 @@
         <v>6.6411042199999999</v>
       </c>
       <c r="L34" s="3">
-        <f t="shared" ref="L34" si="31">1/C34</f>
+        <f>1/C34</f>
         <v>0.18871317840493429</v>
       </c>
-      <c r="M34" s="3"/>
+      <c r="M34" s="3">
+        <f>1/D34</f>
+        <v>0.18590621037263885</v>
+      </c>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3">
-        <f t="shared" ref="R34:S34" si="32">1/I34</f>
+        <f t="shared" ref="R34:S34" si="31">1/I34</f>
         <v>0.15398737068883597</v>
       </c>
       <c r="S34" s="3">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0.15057736889423487</v>
       </c>
     </row>
@@ -16841,7 +16850,9 @@
       <c r="C35" s="8">
         <v>6.5951081899999998E-3</v>
       </c>
-      <c r="D35" s="8"/>
+      <c r="D35" s="8">
+        <v>5.4260630000000001E-3</v>
+      </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
@@ -16853,20 +16864,23 @@
         <v>1.03017753E-2</v>
       </c>
       <c r="L35" s="4">
-        <f t="shared" ref="L35" si="33">1/(C34-C35)</f>
+        <f>1/(C34-C35)</f>
         <v>0.1889483404538774</v>
       </c>
-      <c r="M35" s="4"/>
+      <c r="M35" s="4">
+        <f>1/(D34-D35)</f>
+        <v>0.1860939305426032</v>
+      </c>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="4">
-        <f t="shared" ref="R35:S35" si="34">1/(I34-I35)</f>
+        <f t="shared" ref="R35:S35" si="32">1/(I34-I35)</f>
         <v>0.1542349721932072</v>
       </c>
       <c r="S35" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0.15081130954207511</v>
       </c>
     </row>
@@ -16879,20 +16893,23 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="L36" s="5">
-        <f t="shared" ref="L36" si="35">1/(C34+C35)</f>
+        <f>1/(C34+C35)</f>
         <v>0.18847860098613631</v>
       </c>
-      <c r="M36" s="5"/>
+      <c r="M36" s="5">
+        <f>1/(D34+D35)</f>
+        <v>0.18571886854227027</v>
+      </c>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
       <c r="R36" s="5">
-        <f t="shared" ref="R36:S36" si="36">1/(I34+I35)</f>
+        <f t="shared" ref="R36:S36" si="33">1/(I34+I35)</f>
         <v>0.15374056288570237</v>
       </c>
       <c r="S36" s="5">
-        <f t="shared" si="36"/>
+        <f t="shared" si="33"/>
         <v>0.15034415290641068</v>
       </c>
     </row>
@@ -16906,20 +16923,23 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="L37" s="3">
-        <f t="shared" ref="L37:P37" si="37">L35-L34</f>
+        <f>L35-L34</f>
         <v>2.3516204894311055E-4</v>
       </c>
-      <c r="M37" s="3"/>
+      <c r="M37" s="3">
+        <f>M35-M34</f>
+        <v>1.8772016996435048E-4</v>
+      </c>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
       <c r="Q37" s="3"/>
       <c r="R37" s="3">
-        <f t="shared" ref="R37:S37" si="38">R35-R34</f>
+        <f t="shared" ref="R37:S37" si="34">R35-R34</f>
         <v>2.4760150437122541E-4</v>
       </c>
       <c r="S37" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="34"/>
         <v>2.3394064784024171E-4</v>
       </c>
     </row>
@@ -16931,28 +16951,31 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1" t="e">
-        <f t="shared" ref="I38:J38" si="39">AVERAGE(I36:I37)</f>
+        <f t="shared" ref="I38:J38" si="35">AVERAGE(I36:I37)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J38" s="1" t="e">
-        <f t="shared" si="39"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L38" s="3">
-        <f t="shared" ref="L38:P38" si="40">L34-L36</f>
+        <f>L34-L36</f>
         <v>2.3457741879798211E-4</v>
       </c>
-      <c r="M38" s="3"/>
+      <c r="M38" s="3">
+        <f>M34-M36</f>
+        <v>1.8734183036858698E-4</v>
+      </c>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
       <c r="R38" s="3">
-        <f t="shared" ref="R38:S38" si="41">R34-R36</f>
+        <f t="shared" ref="R38:S38" si="36">R34-R36</f>
         <v>2.4680780313360295E-4</v>
       </c>
       <c r="S38" s="3">
-        <f t="shared" si="41"/>
+        <f t="shared" si="36"/>
         <v>2.3321598782419239E-4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished chap 1 transfer?
</commit_message>
<xml_diff>
--- a/1810_FSE_for-serious-this-time.xlsx
+++ b/1810_FSE_for-serious-this-time.xlsx
@@ -19,7 +19,6 @@
     <sheet name="4000K-paper1 figure dump" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4488,11 +4487,11 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.18871317840493429</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>0.18590621037263885</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17899407161074174</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.15398737068883597</c:v>
@@ -15441,7 +15440,7 @@
   <dimension ref="B2:S44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U37" sqref="U37"/>
+      <selection activeCell="M34" sqref="M34:M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16815,7 +16814,9 @@
       <c r="D34" s="8">
         <v>5.3790564500000002</v>
       </c>
-      <c r="E34" s="8"/>
+      <c r="E34" s="8">
+        <v>5.5867772100000002</v>
+      </c>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="2"/>
@@ -16825,15 +16826,15 @@
       <c r="J34" s="2">
         <v>6.6411042199999999</v>
       </c>
-      <c r="L34" s="3">
-        <f>1/C34</f>
-        <v>0.18871317840493429</v>
-      </c>
+      <c r="L34" s="3"/>
       <c r="M34" s="3">
         <f>1/D34</f>
         <v>0.18590621037263885</v>
       </c>
-      <c r="N34" s="3"/>
+      <c r="N34" s="3">
+        <f>1/E34</f>
+        <v>0.17899407161074174</v>
+      </c>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
@@ -16853,7 +16854,9 @@
       <c r="D35" s="8">
         <v>5.4260630000000001E-3</v>
       </c>
-      <c r="E35" s="8"/>
+      <c r="E35" s="8">
+        <v>1.2703001E-2</v>
+      </c>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="H35" s="2"/>
@@ -16863,15 +16866,15 @@
       <c r="J35" s="2">
         <v>1.03017753E-2</v>
       </c>
-      <c r="L35" s="4">
-        <f>1/(C34-C35)</f>
-        <v>0.1889483404538774</v>
-      </c>
+      <c r="L35" s="4"/>
       <c r="M35" s="4">
         <f>1/(D34-D35)</f>
         <v>0.1860939305426032</v>
       </c>
-      <c r="N35" s="4"/>
+      <c r="N35" s="4">
+        <f>1/(E34-E35)</f>
+        <v>0.17940198901288076</v>
+      </c>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
@@ -16892,15 +16895,15 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
-      <c r="L36" s="5">
-        <f>1/(C34+C35)</f>
-        <v>0.18847860098613631</v>
-      </c>
+      <c r="L36" s="5"/>
       <c r="M36" s="5">
         <f>1/(D34+D35)</f>
         <v>0.18571886854227027</v>
       </c>
-      <c r="N36" s="5"/>
+      <c r="N36" s="5">
+        <f>1/(E34+E35)</f>
+        <v>0.17858800501438185</v>
+      </c>
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
@@ -16922,15 +16925,15 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
-      <c r="L37" s="3">
-        <f>L35-L34</f>
-        <v>2.3516204894311055E-4</v>
-      </c>
+      <c r="L37" s="3"/>
       <c r="M37" s="3">
         <f>M35-M34</f>
         <v>1.8772016996435048E-4</v>
       </c>
-      <c r="N37" s="3"/>
+      <c r="N37" s="3">
+        <f>N35-N34</f>
+        <v>4.0791740213902417E-4</v>
+      </c>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
       <c r="Q37" s="3"/>
@@ -16958,15 +16961,15 @@
         <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L38" s="3">
-        <f>L34-L36</f>
-        <v>2.3457741879798211E-4</v>
-      </c>
+      <c r="L38" s="3"/>
       <c r="M38" s="3">
         <f>M34-M36</f>
         <v>1.8734183036858698E-4</v>
       </c>
-      <c r="N38" s="3"/>
+      <c r="N38" s="3">
+        <f>N34-N36</f>
+        <v>4.0606659635988862E-4</v>
+      </c>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>

</xml_diff>

<commit_message>
bobbie poo'd on floor lol
</commit_message>
<xml_diff>
--- a/1810_FSE_for-serious-this-time.xlsx
+++ b/1810_FSE_for-serious-this-time.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="32">
   <si>
     <t>1x1</t>
   </si>
@@ -110,6 +110,21 @@
   <si>
     <t>copied from 8x8</t>
   </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>kappa</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>p/m</t>
+  </si>
 </sst>
 </file>
 
@@ -175,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -186,6 +201,9 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4361,12 +4379,12 @@
             <c:trendlineType val="linear"/>
             <c:backward val="1.0000000000000002E-2"/>
             <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.2631380718665772E-2"/>
-                  <c:y val="-2.3435252673198449E-2"/>
+                  <c:x val="-6.1091847823954666E-2"/>
+                  <c:y val="-3.9218312511796832E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4487,11 +4505,23 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.18871317840493429</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>0.18590621037263885</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.17899407161074174</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17591040888504619</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17484896926331542</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16321477269703719</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.15398737068883597</c:v>
@@ -5131,12 +5161,12 @@
             <c:trendlineType val="linear"/>
             <c:backward val="1.0000000000000002E-2"/>
             <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.6617429547763927E-2"/>
-                  <c:y val="6.7726934416487333E-2"/>
+                  <c:x val="1.8629128758008387E-2"/>
+                  <c:y val="8.3740779907141738E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -5323,7 +5353,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4000K-kaproc'!$B$40</c:f>
+              <c:f>'4000K-kaproc'!$B$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5361,7 +5391,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'4000K-kaproc'!$L$43</c:f>
+                <c:f>'4000K-kaproc'!$L$44</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
@@ -5373,7 +5403,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'4000K-kaproc'!$L$44</c:f>
+                <c:f>'4000K-kaproc'!$L$45</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
@@ -5399,7 +5429,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'4000K-kaproc'!$B$41</c:f>
+              <c:f>'4000K-kaproc'!$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -5411,7 +5441,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'4000K-kaproc'!$L$40</c:f>
+              <c:f>'4000K-kaproc'!$L$41</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="1"/>
@@ -15437,10 +15467,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:S44"/>
+  <dimension ref="B2:AA45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34:M38"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U34" sqref="U34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15532,11 +15562,11 @@
         <v>16.390884400000001</v>
       </c>
       <c r="L4" s="3">
-        <f>1/C4</f>
+        <f t="shared" ref="L4:S4" si="1">1/C4</f>
         <v>0.15576300671612234</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" ref="M4:S4" si="1">1/D4</f>
+        <f t="shared" si="1"/>
         <v>0.14298833506310135</v>
       </c>
       <c r="N4" s="3">
@@ -15590,11 +15620,11 @@
         <v>9.5667496000000005E-2</v>
       </c>
       <c r="L5" s="4">
-        <f>1/(C4-C5)</f>
+        <f t="shared" ref="L5:S5" si="2">1/(C4-C5)</f>
         <v>0.15719072854626825</v>
       </c>
       <c r="M5" s="4">
-        <f t="shared" ref="M5:S5" si="2">1/(D4-D5)</f>
+        <f t="shared" si="2"/>
         <v>0.14437573751963312</v>
       </c>
       <c r="N5" s="4">
@@ -15632,11 +15662,11 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="L6" s="5">
-        <f>1/(C4+C5)</f>
+        <f t="shared" ref="L6:S6" si="3">1/(C4+C5)</f>
         <v>0.15436098668320666</v>
       </c>
       <c r="M6" s="5">
-        <f t="shared" ref="M6:S6" si="3">1/(D4+D5)</f>
+        <f t="shared" si="3"/>
         <v>0.14162734374969815</v>
       </c>
       <c r="N6" s="5">
@@ -15674,35 +15704,35 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="L7" s="3">
-        <f>L5-L4</f>
+        <f t="shared" ref="L7" si="4">L5-L4</f>
         <v>1.4277218301459171E-3</v>
       </c>
       <c r="M7" s="3">
-        <f t="shared" ref="M7:S7" si="4">M5-M4</f>
+        <f t="shared" ref="M7:S7" si="5">M5-M4</f>
         <v>1.3874024565317666E-3</v>
       </c>
       <c r="N7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3979583413855357E-3</v>
       </c>
       <c r="O7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2044692341186547E-3</v>
       </c>
       <c r="P7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0555627818852192E-3</v>
       </c>
       <c r="Q7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.1318477935009006E-4</v>
       </c>
       <c r="R7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.1059745267598442E-4</v>
       </c>
       <c r="S7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.5818044678598282E-4</v>
       </c>
     </row>
@@ -15712,63 +15742,63 @@
         <v>#DIV/0!</v>
       </c>
       <c r="D8" s="1" t="e">
-        <f t="shared" ref="D8:J8" si="5">AVERAGE(D6:D7)</f>
+        <f t="shared" ref="D8:J8" si="6">AVERAGE(D6:D7)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E8" s="1" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F8" s="1" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G8" s="1" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H8" s="1" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I8" s="1" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J8" s="1" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L8" s="3">
-        <f>L4-L6</f>
+        <f t="shared" ref="L8" si="7">L4-L6</f>
         <v>1.402020032915674E-3</v>
       </c>
       <c r="M8" s="3">
-        <f t="shared" ref="M8:S8" si="6">M4-M6</f>
+        <f t="shared" ref="M8:S8" si="8">M4-M6</f>
         <v>1.3609913134031981E-3</v>
       </c>
       <c r="N8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.3691559548782983E-3</v>
       </c>
       <c r="O8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.1821358864686771E-3</v>
       </c>
       <c r="P8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.0372028992945842E-3</v>
       </c>
       <c r="Q8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7.0356271748439614E-4</v>
       </c>
       <c r="R8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6.0150774197949286E-4</v>
       </c>
       <c r="S8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.5402357678959023E-4</v>
       </c>
     </row>
@@ -15801,35 +15831,35 @@
         <v>10.804334600000001</v>
       </c>
       <c r="L10" s="3">
-        <f>1/C10</f>
+        <f t="shared" ref="L10:S10" si="9">1/C10</f>
         <v>0.17650060932775857</v>
       </c>
       <c r="M10" s="3">
-        <f t="shared" ref="M10:S10" si="7">1/D10</f>
+        <f t="shared" si="9"/>
         <v>0.17080890998647666</v>
       </c>
       <c r="N10" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.15792125921889238</v>
       </c>
       <c r="O10" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.15110385734693413</v>
       </c>
       <c r="P10" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.14689344289866499</v>
       </c>
       <c r="Q10" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.13494548366418729</v>
       </c>
       <c r="R10" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.11553974638043582</v>
       </c>
       <c r="S10" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>9.255544529322518E-2</v>
       </c>
     </row>
@@ -15859,35 +15889,35 @@
         <v>4.6017418999999997E-2</v>
       </c>
       <c r="L11" s="4">
-        <f>1/(C10-C11)</f>
+        <f t="shared" ref="L11:S11" si="10">1/(C10-C11)</f>
         <v>0.17835426629587631</v>
       </c>
       <c r="M11" s="4">
-        <f t="shared" ref="M11:S11" si="8">1/(D10-D11)</f>
+        <f t="shared" si="10"/>
         <v>0.17204700413755117</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.15987270244781032</v>
       </c>
       <c r="O11" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.15213842076390424</v>
       </c>
       <c r="P11" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.14797210382902676</v>
       </c>
       <c r="Q11" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.13575676689341737</v>
       </c>
       <c r="R11" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.11625028757502077</v>
       </c>
       <c r="S11" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>9.2951340174844022E-2</v>
       </c>
     </row>
@@ -15901,35 +15931,35 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="L12" s="5">
-        <f>1/(C10+C11)</f>
+        <f t="shared" ref="L12:S12" si="11">1/(C10+C11)</f>
         <v>0.17468508657808379</v>
       </c>
       <c r="M12" s="5">
-        <f t="shared" ref="M12:S12" si="9">1/(D10+D11)</f>
+        <f t="shared" si="11"/>
         <v>0.16958850780247911</v>
       </c>
       <c r="N12" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.15601688103900979</v>
       </c>
       <c r="O12" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.15008326925948387</v>
       </c>
       <c r="P12" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.14583039422503427</v>
       </c>
       <c r="Q12" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.13414383929964688</v>
       </c>
       <c r="R12" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.11483783831190707</v>
       </c>
       <c r="S12" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>9.2162908470518251E-2</v>
       </c>
     </row>
@@ -15943,35 +15973,35 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="L13" s="3">
-        <f>L11-L10</f>
+        <f t="shared" ref="L13" si="12">L11-L10</f>
         <v>1.8536569681177339E-3</v>
       </c>
       <c r="M13" s="3">
-        <f t="shared" ref="M13:S13" si="10">M11-M10</f>
+        <f t="shared" ref="M13:S13" si="13">M11-M10</f>
         <v>1.2380941510745092E-3</v>
       </c>
       <c r="N13" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1.9514432289179373E-3</v>
       </c>
       <c r="O13" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1.0345634169701134E-3</v>
       </c>
       <c r="P13" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1.0786609303617689E-3</v>
       </c>
       <c r="Q13" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>8.1128322923007534E-4</v>
       </c>
       <c r="R13" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>7.1054119458495435E-4</v>
       </c>
       <c r="S13" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>3.9589488161884123E-4</v>
       </c>
     </row>
@@ -15981,63 +16011,63 @@
         <v>#DIV/0!</v>
       </c>
       <c r="D14" s="1" t="e">
-        <f t="shared" ref="D14:J14" si="11">AVERAGE(D12:D13)</f>
+        <f t="shared" ref="D14:J14" si="14">AVERAGE(D12:D13)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E14" s="1" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F14" s="1" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G14" s="1" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H14" s="1" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I14" s="1" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J14" s="1" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L14" s="3">
-        <f>L10-L12</f>
+        <f t="shared" ref="L14" si="15">L10-L12</f>
         <v>1.8155227496747806E-3</v>
       </c>
       <c r="M14" s="3">
-        <f t="shared" ref="M14:S14" si="12">M10-M12</f>
+        <f t="shared" ref="M14:S14" si="16">M10-M12</f>
         <v>1.2204021839975487E-3</v>
       </c>
       <c r="N14" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.9043781798825932E-3</v>
       </c>
       <c r="O14" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.0205880874502582E-3</v>
       </c>
       <c r="P14" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.0630486736307176E-3</v>
       </c>
       <c r="Q14" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>8.0164436454041588E-4</v>
       </c>
       <c r="R14" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>7.019080685287532E-4</v>
       </c>
       <c r="S14" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>3.9253682270692924E-4</v>
       </c>
     </row>
@@ -16070,35 +16100,35 @@
         <v>7.6483950600000004</v>
       </c>
       <c r="L16" s="3">
-        <f>1/C16</f>
+        <f t="shared" ref="L16:S16" si="17">1/C16</f>
         <v>0.19483135104058588</v>
       </c>
       <c r="M16" s="3">
-        <f t="shared" ref="M16:S16" si="13">1/D16</f>
+        <f t="shared" si="17"/>
         <v>0.18971600314930082</v>
       </c>
       <c r="N16" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.18151130230946996</v>
       </c>
       <c r="O16" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.18109309264820228</v>
       </c>
       <c r="P16" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.17141884208690908</v>
       </c>
       <c r="Q16" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.16780212266262004</v>
       </c>
       <c r="R16" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.14902362840712666</v>
       </c>
       <c r="S16" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.13074638432706689</v>
       </c>
     </row>
@@ -16128,35 +16158,35 @@
         <v>3.2915786000000002E-2</v>
       </c>
       <c r="L17" s="4">
-        <f>1/(C16-C17)</f>
+        <f t="shared" ref="L17:S17" si="18">1/(C16-C17)</f>
         <v>0.19682657675511073</v>
       </c>
       <c r="M17" s="4">
-        <f t="shared" ref="M17:S17" si="14">1/(D16-D17)</f>
+        <f t="shared" si="18"/>
         <v>0.19119238513309197</v>
       </c>
       <c r="N17" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.18271270601990425</v>
       </c>
       <c r="O17" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.18200738799547955</v>
       </c>
       <c r="P17" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.1721417402378172</v>
       </c>
       <c r="Q17" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.16845709402329875</v>
       </c>
       <c r="R17" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.14959208752375264</v>
       </c>
       <c r="S17" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.13131149912180826</v>
       </c>
     </row>
@@ -16170,35 +16200,35 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="L18" s="5">
-        <f>1/(C16+C17)</f>
+        <f t="shared" ref="L18:S18" si="19">1/(C16+C17)</f>
         <v>0.19287617048813535</v>
       </c>
       <c r="M18" s="5">
-        <f t="shared" ref="M18:S18" si="15">1/(D16+D17)</f>
+        <f t="shared" si="19"/>
         <v>0.18826224760148766</v>
       </c>
       <c r="N18" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.18032559473977833</v>
       </c>
       <c r="O18" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.18018793712477507</v>
       </c>
       <c r="P18" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.17070199007408282</v>
       </c>
       <c r="Q18" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.16715222471266852</v>
       </c>
       <c r="R18" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.14845947329410886</v>
       </c>
       <c r="S18" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.13018611276755507</v>
       </c>
     </row>
@@ -16212,35 +16242,35 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="L19" s="3">
-        <f>L17-L16</f>
+        <f t="shared" ref="L19" si="20">L17-L16</f>
         <v>1.9952257145248453E-3</v>
       </c>
       <c r="M19" s="3">
-        <f t="shared" ref="M19:S19" si="16">M17-M16</f>
+        <f t="shared" ref="M19:S19" si="21">M17-M16</f>
         <v>1.4763819837911585E-3</v>
       </c>
       <c r="N19" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>1.2014037104342845E-3</v>
       </c>
       <c r="O19" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>9.1429534727727191E-4</v>
       </c>
       <c r="P19" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>7.2289815090811893E-4</v>
       </c>
       <c r="Q19" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>6.5497136067871331E-4</v>
       </c>
       <c r="R19" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>5.6845911662598003E-4</v>
       </c>
       <c r="S19" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>5.651147947413615E-4</v>
       </c>
     </row>
@@ -16250,63 +16280,63 @@
         <v>#DIV/0!</v>
       </c>
       <c r="D20" s="1" t="e">
-        <f t="shared" ref="D20:J20" si="17">AVERAGE(D18:D19)</f>
+        <f t="shared" ref="D20:J20" si="22">AVERAGE(D18:D19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E20" s="1" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F20" s="1" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G20" s="1" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H20" s="1" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I20" s="1" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J20" s="1" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L20" s="3">
-        <f>L16-L18</f>
+        <f t="shared" ref="L20" si="23">L16-L18</f>
         <v>1.9551805524505306E-3</v>
       </c>
       <c r="M20" s="3">
-        <f t="shared" ref="M20:S20" si="18">M16-M18</f>
+        <f t="shared" ref="M20:S20" si="24">M16-M18</f>
         <v>1.453755547813157E-3</v>
       </c>
       <c r="N20" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1.1857075696916353E-3</v>
       </c>
       <c r="O20" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>9.0515552342720906E-4</v>
       </c>
       <c r="P20" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>7.1685201282625788E-4</v>
       </c>
       <c r="Q20" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>6.4989794995151673E-4</v>
       </c>
       <c r="R20" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>5.6415511301780019E-4</v>
       </c>
       <c r="S20" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>5.6027155951182683E-4</v>
       </c>
     </row>
@@ -16337,31 +16367,31 @@
       </c>
       <c r="J22" s="2"/>
       <c r="L22" s="3">
-        <f>1/C22</f>
+        <f t="shared" ref="L22:R22" si="25">1/C22</f>
         <v>0.18127786895712172</v>
       </c>
       <c r="M22" s="3">
-        <f t="shared" ref="M22:R22" si="19">1/D22</f>
+        <f t="shared" si="25"/>
         <v>0.17686045275908038</v>
       </c>
       <c r="N22" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.17111671131997178</v>
       </c>
       <c r="O22" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.16801856927786174</v>
       </c>
       <c r="P22" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.16008237890444785</v>
       </c>
       <c r="Q22" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.15375157817538659</v>
       </c>
       <c r="R22" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.14455737841863636</v>
       </c>
       <c r="S22" s="3"/>
@@ -16390,31 +16420,31 @@
       </c>
       <c r="J23" s="2"/>
       <c r="L23" s="4">
-        <f>1/(C22-C23)</f>
+        <f t="shared" ref="L23:R23" si="26">1/(C22-C23)</f>
         <v>0.18256650662645102</v>
       </c>
       <c r="M23" s="4">
-        <f t="shared" ref="M23:R23" si="20">1/(D22-D23)</f>
+        <f t="shared" si="26"/>
         <v>0.17780900467420491</v>
       </c>
       <c r="N23" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>0.17225870728249168</v>
       </c>
       <c r="O23" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>0.1688420596461567</v>
       </c>
       <c r="P23" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>0.16070504024140106</v>
       </c>
       <c r="Q23" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>0.15412607206970824</v>
       </c>
       <c r="R23" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>0.14491812100657539</v>
       </c>
       <c r="S23" s="4"/>
@@ -16429,31 +16459,31 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="L24" s="5">
-        <f>1/(C22+C23)</f>
+        <f t="shared" ref="L24:R24" si="27">1/(C22+C23)</f>
         <v>0.180007295368068</v>
       </c>
       <c r="M24" s="5">
-        <f t="shared" ref="M24:R24" si="21">1/(D22+D23)</f>
+        <f t="shared" si="27"/>
         <v>0.1759219675594878</v>
       </c>
       <c r="N24" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>0.16998975745075373</v>
       </c>
       <c r="O24" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>0.16720307271133289</v>
       </c>
       <c r="P24" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>0.15946452402214245</v>
       </c>
       <c r="Q24" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>0.15337889975243243</v>
       </c>
       <c r="R24" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>0.14419842735372462</v>
       </c>
       <c r="S24" s="5"/>
@@ -16468,31 +16498,31 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="L25" s="3">
-        <f>L23-L22</f>
+        <f t="shared" ref="L25" si="28">L23-L22</f>
         <v>1.2886376693292956E-3</v>
       </c>
       <c r="M25" s="3">
-        <f t="shared" ref="M25:R25" si="22">M23-M22</f>
+        <f t="shared" ref="M25:R25" si="29">M23-M22</f>
         <v>9.4855191512452364E-4</v>
       </c>
       <c r="N25" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>1.1419959625199039E-3</v>
       </c>
       <c r="O25" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>8.2349036829496014E-4</v>
       </c>
       <c r="P25" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>6.2266133695321191E-4</v>
       </c>
       <c r="Q25" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>3.7449389432164804E-4</v>
       </c>
       <c r="R25" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>3.6074258793902803E-4</v>
       </c>
       <c r="S25" s="3"/>
@@ -16503,56 +16533,56 @@
         <v>#DIV/0!</v>
       </c>
       <c r="D26" s="1" t="e">
-        <f t="shared" ref="D26:I26" si="23">AVERAGE(D24:D25)</f>
+        <f t="shared" ref="D26:I26" si="30">AVERAGE(D24:D25)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E26" s="1" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F26" s="1" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G26" s="1" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H26" s="1" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I26" s="1" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J26" s="1"/>
       <c r="L26" s="3">
-        <f>L22-L24</f>
+        <f t="shared" ref="L26" si="31">L22-L24</f>
         <v>1.2705735890537195E-3</v>
       </c>
       <c r="M26" s="3">
-        <f t="shared" ref="M26:R26" si="24">M22-M24</f>
+        <f t="shared" ref="M26:R26" si="32">M22-M24</f>
         <v>9.3848519959258137E-4</v>
       </c>
       <c r="N26" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>1.1269538692180447E-3</v>
       </c>
       <c r="O26" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>8.154965665288505E-4</v>
       </c>
       <c r="P26" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>6.1785488230539642E-4</v>
       </c>
       <c r="Q26" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>3.7267842295415909E-4</v>
       </c>
       <c r="R26" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>3.5895106491173889E-4</v>
       </c>
       <c r="S26" s="3"/>
@@ -16584,31 +16614,31 @@
       </c>
       <c r="J28" s="2"/>
       <c r="L28" s="3">
-        <f>1/C28</f>
+        <f t="shared" ref="L28:R28" si="33">1/C28</f>
         <v>0.18311914076660976</v>
       </c>
       <c r="M28" s="3">
-        <f t="shared" ref="M28:R28" si="25">1/D28</f>
+        <f t="shared" si="33"/>
         <v>0.17417258455905243</v>
       </c>
       <c r="N28" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>0.17209020625119636</v>
       </c>
       <c r="O28" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>0.16790992661389195</v>
       </c>
       <c r="P28" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>0.16229090780249633</v>
       </c>
       <c r="Q28" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>0.15344388888805774</v>
       </c>
       <c r="R28" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="33"/>
         <v>0.14313379553774153</v>
       </c>
       <c r="S28" s="3"/>
@@ -16637,31 +16667,31 @@
       </c>
       <c r="J29" s="2"/>
       <c r="L29" s="4">
-        <f>1/(C28-C29)</f>
+        <f t="shared" ref="L29:R29" si="34">1/(C28-C29)</f>
         <v>0.18386219634141748</v>
       </c>
       <c r="M29" s="4">
-        <f t="shared" ref="M29:R29" si="26">1/(D28-D29)</f>
+        <f t="shared" si="34"/>
         <v>0.17462513352245898</v>
       </c>
       <c r="N29" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="34"/>
         <v>0.17279650172293423</v>
       </c>
       <c r="O29" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="34"/>
         <v>0.16841435312988484</v>
       </c>
       <c r="P29" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="34"/>
         <v>0.16283088517754221</v>
       </c>
       <c r="Q29" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="34"/>
         <v>0.15402727933431348</v>
       </c>
       <c r="R29" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="34"/>
         <v>0.14380492175551557</v>
       </c>
       <c r="S29" s="4"/>
@@ -16676,31 +16706,31 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="L30" s="5">
-        <f>1/(C28+C29)</f>
+        <f t="shared" ref="L30:R30" si="35">1/(C28+C29)</f>
         <v>0.18238206694564191</v>
       </c>
       <c r="M30" s="5">
-        <f t="shared" ref="M30:R30" si="27">1/(D28+D29)</f>
+        <f t="shared" si="35"/>
         <v>0.17372237513500208</v>
       </c>
       <c r="N30" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="35"/>
         <v>0.17138966115699089</v>
       </c>
       <c r="O30" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="35"/>
         <v>0.16740851274232582</v>
       </c>
       <c r="P30" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="35"/>
         <v>0.16175449992033317</v>
       </c>
       <c r="Q30" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="35"/>
         <v>0.15286490104109562</v>
       </c>
       <c r="R30" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="35"/>
         <v>0.14246890440746468</v>
       </c>
       <c r="S30" s="5"/>
@@ -16715,31 +16745,31 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="L31" s="3">
-        <f>L29-L28</f>
+        <f t="shared" ref="L31" si="36">L29-L28</f>
         <v>7.4305557480772166E-4</v>
       </c>
       <c r="M31" s="3">
-        <f t="shared" ref="M31:R31" si="28">M29-M28</f>
+        <f t="shared" ref="M31:R31" si="37">M29-M28</f>
         <v>4.5254896340654605E-4</v>
       </c>
       <c r="N31" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="37"/>
         <v>7.0629547173786666E-4</v>
       </c>
       <c r="O31" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="37"/>
         <v>5.0442651599288957E-4</v>
       </c>
       <c r="P31" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="37"/>
         <v>5.3997737504588028E-4</v>
       </c>
       <c r="Q31" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="37"/>
         <v>5.8339044625574377E-4</v>
       </c>
       <c r="R31" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="37"/>
         <v>6.7112621777404291E-4</v>
       </c>
       <c r="S31" s="3"/>
@@ -16750,61 +16780,81 @@
         <v>#DIV/0!</v>
       </c>
       <c r="D32" s="1" t="e">
-        <f t="shared" ref="D32:I32" si="29">AVERAGE(D30:D31)</f>
+        <f t="shared" ref="D32:I32" si="38">AVERAGE(D30:D31)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E32" s="1" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F32" s="1" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G32" s="1" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H32" s="1" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I32" s="1" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J32" s="1"/>
       <c r="L32" s="3">
-        <f>L28-L30</f>
+        <f t="shared" ref="L32" si="39">L28-L30</f>
         <v>7.3707382096785401E-4</v>
       </c>
       <c r="M32" s="3">
-        <f t="shared" ref="M32:R32" si="30">M28-M30</f>
+        <f t="shared" ref="M32:R32" si="40">M28-M30</f>
         <v>4.5020942405035735E-4</v>
       </c>
       <c r="N32" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>7.0054509420547362E-4</v>
       </c>
       <c r="O32" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>5.0141387156613093E-4</v>
       </c>
       <c r="P32" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>5.364078821631646E-4</v>
       </c>
       <c r="Q32" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>5.7898784696211458E-4</v>
       </c>
       <c r="R32" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="40"/>
         <v>6.6489113027684565E-4</v>
       </c>
       <c r="S32" s="3"/>
     </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="U33" t="s">
+        <v>27</v>
+      </c>
+      <c r="V33" t="s">
+        <v>28</v>
+      </c>
+      <c r="X33" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>24</v>
       </c>
@@ -16817,16 +16867,25 @@
       <c r="E34" s="8">
         <v>5.5867772100000002</v>
       </c>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="2"/>
+      <c r="F34" s="8">
+        <v>5.6847119299999997</v>
+      </c>
+      <c r="G34" s="8">
+        <v>5.7192215900000001</v>
+      </c>
+      <c r="H34" s="2">
+        <v>6.1268963799999998</v>
+      </c>
       <c r="I34" s="2">
         <v>6.4940390600000004</v>
       </c>
       <c r="J34" s="2">
         <v>6.6411042199999999</v>
       </c>
-      <c r="L34" s="3"/>
+      <c r="L34" s="3">
+        <f>1/C34</f>
+        <v>0.18871317840493429</v>
+      </c>
       <c r="M34" s="3">
         <f>1/D34</f>
         <v>0.18590621037263885</v>
@@ -16835,38 +16894,75 @@
         <f>1/E34</f>
         <v>0.17899407161074174</v>
       </c>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
+      <c r="O34" s="3">
+        <f t="shared" ref="O34:Q34" si="41">1/F34</f>
+        <v>0.17591040888504619</v>
+      </c>
+      <c r="P34" s="3">
+        <f t="shared" si="41"/>
+        <v>0.17484896926331542</v>
+      </c>
+      <c r="Q34" s="3">
+        <f t="shared" si="41"/>
+        <v>0.16321477269703719</v>
+      </c>
       <c r="R34" s="3">
-        <f t="shared" ref="R34:S34" si="31">1/I34</f>
+        <f t="shared" ref="R34:S34" si="42">1/I34</f>
         <v>0.15398737068883597</v>
       </c>
       <c r="S34" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="42"/>
         <v>0.15057736889423487</v>
       </c>
+      <c r="U34">
+        <f t="array" ref="U34:V35">LINEST(U38:AA38,U37:AA37,1,1)</f>
+        <v>0.30879410101658622</v>
+      </c>
+      <c r="V34">
+        <v>0.14948739858367716</v>
+      </c>
+      <c r="X34" s="2">
+        <f>1/V34</f>
+        <v>6.6895270736833341</v>
+      </c>
+      <c r="Y34" s="2">
+        <f>1/(V34-V35)</f>
+        <v>6.7962429550833772</v>
+      </c>
+      <c r="Z34" s="2">
+        <f>1/(V34+V35)</f>
+        <v>6.5861107279209072</v>
+      </c>
     </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="C35" s="8">
+    <row r="35" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="C35" s="10">
         <v>6.5951081899999998E-3</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="10">
         <v>5.4260630000000001E-3</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="10">
         <v>1.2703001E-2</v>
       </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2">
+      <c r="F35" s="10">
+        <v>8.3924099999999995E-3</v>
+      </c>
+      <c r="G35" s="10">
+        <v>1.1307315E-2</v>
+      </c>
+      <c r="H35" s="11">
+        <v>8.4161240000000005E-3</v>
+      </c>
+      <c r="I35" s="11">
         <v>1.0425222099999999E-2</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J35" s="11">
         <v>1.03017753E-2</v>
       </c>
-      <c r="L35" s="4"/>
+      <c r="L35" s="4">
+        <f>1/(C34-C35)</f>
+        <v>0.1889483404538774</v>
+      </c>
       <c r="M35" s="4">
         <f>1/(D34-D35)</f>
         <v>0.1860939305426032</v>
@@ -16875,27 +16971,66 @@
         <f>1/(E34-E35)</f>
         <v>0.17940198901288076</v>
       </c>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
+      <c r="O35" s="4">
+        <f t="shared" ref="O35:Q35" si="43">1/(F34-F35)</f>
+        <v>0.17617049154414058</v>
+      </c>
+      <c r="P35" s="4">
+        <f t="shared" si="43"/>
+        <v>0.17519534313608801</v>
+      </c>
+      <c r="Q35" s="4">
+        <f t="shared" si="43"/>
+        <v>0.16343927873582076</v>
+      </c>
       <c r="R35" s="4">
-        <f t="shared" ref="R35:S35" si="32">1/(I34-I35)</f>
+        <f t="shared" ref="R35:S35" si="44">1/(I34-I35)</f>
         <v>0.1542349721932072</v>
       </c>
       <c r="S35" s="4">
-        <f t="shared" si="32"/>
+        <f t="shared" si="44"/>
         <v>0.15081130954207511</v>
       </c>
+      <c r="U35">
+        <v>3.1546674884902128E-2</v>
+      </c>
+      <c r="V35">
+        <v>2.3472791663700998E-3</v>
+      </c>
+      <c r="X35" s="2">
+        <f>(Y34-Z34)/2</f>
+        <v>0.10506611358123497</v>
+      </c>
     </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="L36" s="5"/>
+    <row r="36" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="C36" s="1">
+        <v>3649.3515600000001</v>
+      </c>
+      <c r="D36" s="9">
+        <v>3514.5183099999999</v>
+      </c>
+      <c r="E36" s="9">
+        <v>3707.1743200000001</v>
+      </c>
+      <c r="F36" s="9">
+        <v>3628.7241199999999</v>
+      </c>
+      <c r="G36" s="9">
+        <v>3747.6955600000001</v>
+      </c>
+      <c r="H36" s="1">
+        <v>3704.4086900000002</v>
+      </c>
+      <c r="I36" s="1">
+        <v>3672.0717800000002</v>
+      </c>
+      <c r="J36" s="1">
+        <v>3493.6738300000002</v>
+      </c>
+      <c r="L36" s="5">
+        <f>1/(C34+C35)</f>
+        <v>0.18847860098613631</v>
+      </c>
       <c r="M36" s="5">
         <f>1/(D34+D35)</f>
         <v>0.18571886854227027</v>
@@ -16904,28 +17039,56 @@
         <f>1/(E34+E35)</f>
         <v>0.17858800501438185</v>
       </c>
-      <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="5"/>
+      <c r="O36" s="5">
+        <f t="shared" ref="O36:Q36" si="45">1/(F34+F35)</f>
+        <v>0.17565109302036788</v>
+      </c>
+      <c r="P36" s="5">
+        <f t="shared" si="45"/>
+        <v>0.17450396230049206</v>
+      </c>
+      <c r="Q36" s="5">
+        <f t="shared" si="45"/>
+        <v>0.16299088259123501</v>
+      </c>
       <c r="R36" s="5">
-        <f t="shared" ref="R36:S36" si="33">1/(I34+I35)</f>
+        <f t="shared" ref="R36:S36" si="46">1/(I34+I35)</f>
         <v>0.15374056288570237</v>
       </c>
       <c r="S36" s="5">
-        <f t="shared" si="33"/>
+        <f t="shared" si="46"/>
         <v>0.15034415290641068</v>
       </c>
     </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="L37" s="3"/>
+    <row r="37" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="C37" s="12">
+        <v>4342.2587899999999</v>
+      </c>
+      <c r="D37" s="12">
+        <v>4502.5898399999996</v>
+      </c>
+      <c r="E37" s="12">
+        <v>4255.4453100000001</v>
+      </c>
+      <c r="F37" s="12">
+        <v>4335.6992200000004</v>
+      </c>
+      <c r="G37" s="12">
+        <v>4241.9604499999996</v>
+      </c>
+      <c r="H37" s="12">
+        <v>4296.5781299999999</v>
+      </c>
+      <c r="I37" s="12">
+        <v>4371.4628899999998</v>
+      </c>
+      <c r="J37" s="12">
+        <v>4513.8500999999997</v>
+      </c>
+      <c r="L37" s="3">
+        <f>L35-L34</f>
+        <v>2.3516204894311055E-4</v>
+      </c>
       <c r="M37" s="3">
         <f>M35-M34</f>
         <v>1.8772016996435048E-4</v>
@@ -16934,34 +17097,92 @@
         <f>N35-N34</f>
         <v>4.0791740213902417E-4</v>
       </c>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
+      <c r="O37" s="3">
+        <f t="shared" ref="O37:Q37" si="47">O35-O34</f>
+        <v>2.6008265909438499E-4</v>
+      </c>
+      <c r="P37" s="3">
+        <f t="shared" ref="P37" si="48">P35-P34</f>
+        <v>3.4637387277258735E-4</v>
+      </c>
+      <c r="Q37" s="3">
+        <f t="shared" si="47"/>
+        <v>2.2450603878357289E-4</v>
+      </c>
       <c r="R37" s="3">
-        <f t="shared" ref="R37:S37" si="34">R35-R34</f>
+        <f t="shared" ref="R37:S37" si="49">R35-R34</f>
         <v>2.4760150437122541E-4</v>
       </c>
       <c r="S37" s="3">
-        <f t="shared" si="34"/>
+        <f t="shared" si="49"/>
         <v>2.3394064784024171E-4</v>
       </c>
+      <c r="U37">
+        <f>M2</f>
+        <v>0.125</v>
+      </c>
+      <c r="V37">
+        <f>N2</f>
+        <v>0.1</v>
+      </c>
+      <c r="W37">
+        <f>O2</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="X37">
+        <f>P2</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="Y37">
+        <f>Q2</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z37">
+        <f>R2</f>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="AA37">
+        <f>S2</f>
+        <v>1.0416666666666666E-2</v>
+      </c>
     </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1" t="e">
-        <f t="shared" ref="I38:J38" si="35">AVERAGE(I36:I37)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J38" s="1" t="e">
-        <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L38" s="3"/>
+    <row r="38" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="C38" s="1">
+        <f t="shared" ref="C38:H38" si="50">AVERAGE(C36:C37)</f>
+        <v>3995.805175</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="50"/>
+        <v>4008.554075</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="50"/>
+        <v>3981.3098150000001</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="50"/>
+        <v>3982.2116700000001</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="50"/>
+        <v>3994.8280049999998</v>
+      </c>
+      <c r="H38" s="1">
+        <f t="shared" si="50"/>
+        <v>4000.49341</v>
+      </c>
+      <c r="I38" s="1">
+        <f t="shared" ref="I38:J38" si="51">AVERAGE(I36:I37)</f>
+        <v>4021.767335</v>
+      </c>
+      <c r="J38" s="1">
+        <f t="shared" si="51"/>
+        <v>4003.7619649999997</v>
+      </c>
+      <c r="L38" s="3">
+        <f>L34-L36</f>
+        <v>2.3457741879798211E-4</v>
+      </c>
       <c r="M38" s="3">
         <f>M34-M36</f>
         <v>1.8734183036858698E-4</v>
@@ -16970,57 +17191,143 @@
         <f>N34-N36</f>
         <v>4.0606659635988862E-4</v>
       </c>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
+      <c r="O38" s="3">
+        <f t="shared" ref="O38:Q38" si="52">O34-O36</f>
+        <v>2.5931586467831114E-4</v>
+      </c>
+      <c r="P38" s="3">
+        <f t="shared" ref="P38" si="53">P34-P36</f>
+        <v>3.4500696282335763E-4</v>
+      </c>
+      <c r="Q38" s="3">
+        <f t="shared" si="52"/>
+        <v>2.2389010580217694E-4</v>
+      </c>
       <c r="R38" s="3">
-        <f t="shared" ref="R38:S38" si="36">R34-R36</f>
+        <f t="shared" ref="R38:S38" si="54">R34-R36</f>
         <v>2.4680780313360295E-4</v>
       </c>
       <c r="S38" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="54"/>
         <v>2.3321598782419239E-4</v>
       </c>
+      <c r="U38" s="3">
+        <f>M34</f>
+        <v>0.18590621037263885</v>
+      </c>
+      <c r="V38" s="3">
+        <f>N34</f>
+        <v>0.17899407161074174</v>
+      </c>
+      <c r="W38" s="3">
+        <f>O34</f>
+        <v>0.17591040888504619</v>
+      </c>
+      <c r="X38" s="3">
+        <f>P34</f>
+        <v>0.17484896926331542</v>
+      </c>
+      <c r="Y38" s="3">
+        <f>Q34</f>
+        <v>0.16321477269703719</v>
+      </c>
+      <c r="Z38" s="3">
+        <f>R34</f>
+        <v>0.15398737068883597</v>
+      </c>
+      <c r="AA38" s="3">
+        <f>S34</f>
+        <v>0.15057736889423487</v>
+      </c>
     </row>
-    <row r="40" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+    <row r="39" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="C39" s="1">
+        <f>(C37-C36)/2</f>
+        <v>346.4536149999999</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" ref="D39:J39" si="55">(D37-D36)/2</f>
+        <v>494.03576499999986</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="55"/>
+        <v>274.13549499999999</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="55"/>
+        <v>353.48755000000028</v>
+      </c>
+      <c r="G39" s="1">
+        <f t="shared" si="55"/>
+        <v>247.13244499999973</v>
+      </c>
+      <c r="H39" s="1">
+        <f t="shared" si="55"/>
+        <v>296.08471999999983</v>
+      </c>
+      <c r="I39" s="1">
+        <f t="shared" si="55"/>
+        <v>349.69555499999979</v>
+      </c>
+      <c r="J39" s="1">
+        <f t="shared" si="55"/>
+        <v>510.08813499999974</v>
+      </c>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Y39" s="3"/>
+      <c r="Z39" s="3"/>
+      <c r="AA39" s="3"/>
+    </row>
+    <row r="41" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>25</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <v>7.07</v>
       </c>
-      <c r="L40" s="3">
-        <f>1/C40</f>
+      <c r="L41" s="3">
+        <f>1/C41</f>
         <v>0.14144271570014144</v>
       </c>
     </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B41">
+    <row r="42" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B42">
         <v>0</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <v>0.06</v>
       </c>
-      <c r="L41" s="4">
-        <f>1/(C40-C41)</f>
+      <c r="L42" s="4">
+        <f>1/(C41-C42)</f>
         <v>0.14265335235378029</v>
       </c>
     </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="L42" s="5">
-        <f>1/(C40+C41)</f>
+    <row r="43" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="L43" s="5">
+        <f>1/(C41+C42)</f>
         <v>0.14025245441795231</v>
       </c>
     </row>
-    <row r="43" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="L43" s="3">
-        <f>L41-L40</f>
+    <row r="44" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="L44" s="3">
+        <f>L42-L41</f>
         <v>1.2106366536388524E-3</v>
       </c>
     </row>
-    <row r="44" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="L44" s="3">
-        <f>L40-L42</f>
+    <row r="45" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="L45" s="3">
+        <f>L41-L43</f>
         <v>1.1902612821891312E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished tasks up to 5, first draft
</commit_message>
<xml_diff>
--- a/1810_FSE_for-serious-this-time.xlsx
+++ b/1810_FSE_for-serious-this-time.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
   <si>
     <t>1x1</t>
   </si>
@@ -124,6 +124,15 @@
   </si>
   <si>
     <t>p/m</t>
+  </si>
+  <si>
+    <t>orig_16</t>
+  </si>
+  <si>
+    <t>redo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -4518,7 +4527,7 @@
                   <c:v>0.17591040888504619</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17484896926331542</c:v>
+                  <c:v>0.17402132136028589</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.16321477269703719</c:v>
@@ -15467,10 +15476,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AA45"/>
+  <dimension ref="B2:AA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U34" sqref="U34"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16835,6 +16844,9 @@
       <c r="S32" s="3"/>
     </row>
     <row r="33" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>33</v>
+      </c>
       <c r="U33" t="s">
         <v>27</v>
       </c>
@@ -16871,7 +16883,7 @@
         <v>5.6847119299999997</v>
       </c>
       <c r="G34" s="8">
-        <v>5.7192215900000001</v>
+        <v>5.7464222899999999</v>
       </c>
       <c r="H34" s="2">
         <v>6.1268963799999998</v>
@@ -16900,7 +16912,7 @@
       </c>
       <c r="P34" s="3">
         <f t="shared" si="41"/>
-        <v>0.17484896926331542</v>
+        <v>0.17402132136028589</v>
       </c>
       <c r="Q34" s="3">
         <f t="shared" si="41"/>
@@ -16916,22 +16928,22 @@
       </c>
       <c r="U34">
         <f t="array" ref="U34:V35">LINEST(U38:AA38,U37:AA37,1,1)</f>
-        <v>0.30879410101658622</v>
+        <v>0.30886365937892796</v>
       </c>
       <c r="V34">
-        <v>0.14948739858367716</v>
+        <v>0.14936475366563168</v>
       </c>
       <c r="X34" s="2">
         <f>1/V34</f>
-        <v>6.6895270736833341</v>
+        <v>6.6950199123857734</v>
       </c>
       <c r="Y34" s="2">
         <f>1/(V34-V35)</f>
-        <v>6.7962429550833772</v>
+        <v>6.7917466268325466</v>
       </c>
       <c r="Z34" s="2">
         <f>1/(V34+V35)</f>
-        <v>6.5861107279209072</v>
+        <v>6.6010096364948696</v>
       </c>
     </row>
     <row r="35" spans="2:27" x14ac:dyDescent="0.2">
@@ -16948,7 +16960,7 @@
         <v>8.3924099999999995E-3</v>
       </c>
       <c r="G35" s="10">
-        <v>1.1307315E-2</v>
+        <v>6.8579610000000001E-3</v>
       </c>
       <c r="H35" s="11">
         <v>8.4161240000000005E-3</v>
@@ -16977,7 +16989,7 @@
       </c>
       <c r="P35" s="4">
         <f t="shared" si="43"/>
-        <v>0.17519534313608801</v>
+        <v>0.17422925202656092</v>
       </c>
       <c r="Q35" s="4">
         <f t="shared" si="43"/>
@@ -16992,14 +17004,14 @@
         <v>0.15081130954207511</v>
       </c>
       <c r="U35">
-        <v>3.1546674884902128E-2</v>
+        <v>2.8589195423102058E-2</v>
       </c>
       <c r="V35">
-        <v>2.3472791663700998E-3</v>
+        <v>2.1272233300266906E-3</v>
       </c>
       <c r="X35" s="2">
         <f>(Y34-Z34)/2</f>
-        <v>0.10506611358123497</v>
+        <v>9.5368495168838496E-2</v>
       </c>
     </row>
     <row r="36" spans="2:27" x14ac:dyDescent="0.2">
@@ -17016,7 +17028,7 @@
         <v>3628.7241199999999</v>
       </c>
       <c r="G36" s="9">
-        <v>3747.6955600000001</v>
+        <v>3573.08691</v>
       </c>
       <c r="H36" s="1">
         <v>3704.4086900000002</v>
@@ -17045,7 +17057,7 @@
       </c>
       <c r="P36" s="5">
         <f t="shared" si="45"/>
-        <v>0.17450396230049206</v>
+        <v>0.1738138864044014</v>
       </c>
       <c r="Q36" s="5">
         <f t="shared" si="45"/>
@@ -17074,7 +17086,7 @@
         <v>4335.6992200000004</v>
       </c>
       <c r="G37" s="12">
-        <v>4241.9604499999996</v>
+        <v>4414.7304700000004</v>
       </c>
       <c r="H37" s="12">
         <v>4296.5781299999999</v>
@@ -17103,7 +17115,7 @@
       </c>
       <c r="P37" s="3">
         <f t="shared" ref="P37" si="48">P35-P34</f>
-        <v>3.4637387277258735E-4</v>
+        <v>2.0793066627503021E-4</v>
       </c>
       <c r="Q37" s="3">
         <f t="shared" si="47"/>
@@ -17165,7 +17177,7 @@
       </c>
       <c r="G38" s="1">
         <f t="shared" si="51"/>
-        <v>3994.8280049999998</v>
+        <v>3993.9086900000002</v>
       </c>
       <c r="H38" s="1">
         <f t="shared" si="51"/>
@@ -17197,7 +17209,7 @@
       </c>
       <c r="P38" s="3">
         <f t="shared" ref="P38" si="54">P34-P36</f>
-        <v>3.4500696282335763E-4</v>
+        <v>2.0743495588448901E-4</v>
       </c>
       <c r="Q38" s="3">
         <f t="shared" si="53"/>
@@ -17225,7 +17237,7 @@
       </c>
       <c r="X38" s="3">
         <f t="shared" si="56"/>
-        <v>0.17484896926331542</v>
+        <v>0.17402132136028589</v>
       </c>
       <c r="Y38" s="3">
         <f t="shared" si="56"/>
@@ -17259,7 +17271,7 @@
       </c>
       <c r="G39" s="1">
         <f t="shared" si="57"/>
-        <v>247.13244499999973</v>
+        <v>420.82178000000022</v>
       </c>
       <c r="H39" s="1">
         <f t="shared" si="57"/>
@@ -17296,6 +17308,9 @@
       <c r="C41">
         <v>7.07</v>
       </c>
+      <c r="G41" t="s">
+        <v>32</v>
+      </c>
       <c r="L41" s="3">
         <f>1/C41</f>
         <v>0.14144271570014144</v>
@@ -17308,27 +17323,52 @@
       <c r="C42">
         <v>0.06</v>
       </c>
+      <c r="G42" s="2">
+        <v>5.7192215900000001</v>
+      </c>
       <c r="L42" s="4">
         <f>1/(C41-C42)</f>
         <v>0.14265335235378029</v>
       </c>
     </row>
     <row r="43" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="G43" s="2">
+        <v>1.1307315E-2</v>
+      </c>
       <c r="L43" s="5">
         <f>1/(C41+C42)</f>
         <v>0.14025245441795231</v>
       </c>
     </row>
     <row r="44" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="G44" s="1">
+        <v>3747.6955600000001</v>
+      </c>
+      <c r="H44" t="s">
+        <v>34</v>
+      </c>
       <c r="L44" s="3">
         <f>L42-L41</f>
         <v>1.2106366536388524E-3</v>
       </c>
     </row>
     <row r="45" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="G45" s="1">
+        <v>4241.9604499999996</v>
+      </c>
       <c r="L45" s="3">
         <f>L41-L43</f>
         <v>1.1902612821891312E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="G46" s="1">
+        <v>3994.8280049999998</v>
+      </c>
+    </row>
+    <row r="47" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="G47" s="1">
+        <v>247.13244499999973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chapter 3 mostly first drafted!
</commit_message>
<xml_diff>
--- a/1810_FSE_for-serious-this-time.xlsx
+++ b/1810_FSE_for-serious-this-time.xlsx
@@ -222,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -236,6 +236,7 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7420,7 +7421,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8868,7 +8868,6 @@
         <c:idx val="15"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8975,7 +8974,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9659,7 +9657,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9777,7 +9774,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -28565,8 +28561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AP57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AM14" sqref="AM14"/>
+    <sheetView tabSelected="1" topLeftCell="T16" workbookViewId="0">
+      <selection activeCell="AA33" sqref="AA33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -28792,7 +28788,7 @@
       <c r="J7" s="1"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3">
-        <f t="shared" ref="L7:Q7" si="19">M5-M4</f>
+        <f t="shared" ref="M7:Q7" si="19">M5-M4</f>
         <v>8.9157310799145573E-4</v>
       </c>
       <c r="N7" s="3">
@@ -28855,7 +28851,7 @@
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3">
-        <f t="shared" ref="L8:Q8" si="22">M4-M6</f>
+        <f t="shared" ref="M8:Q8" si="22">M4-M6</f>
         <v>8.7734240898308669E-4</v>
       </c>
       <c r="N8" s="3">
@@ -29046,7 +29042,7 @@
       <c r="J13" s="1"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3">
-        <f t="shared" ref="L13:Q13" si="42">M11-M10</f>
+        <f t="shared" ref="M13:Q13" si="42">M11-M10</f>
         <v>5.3361484006073101E-4</v>
       </c>
       <c r="N13" s="3">
@@ -29109,7 +29105,7 @@
       </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3">
-        <f t="shared" ref="L14:Q14" si="45">M10-M12</f>
+        <f t="shared" ref="M14:Q14" si="45">M10-M12</f>
         <v>5.2965853279179909E-4</v>
       </c>
       <c r="N14" s="3">
@@ -29300,7 +29296,7 @@
       <c r="J19" s="1"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3">
-        <f t="shared" ref="L19:Q19" si="65">M17-M16</f>
+        <f t="shared" ref="M19:Q19" si="65">M17-M16</f>
         <v>4.2358722540139504E-4</v>
       </c>
       <c r="N19" s="3">
@@ -29363,7 +29359,7 @@
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3">
-        <f t="shared" ref="L20:Q20" si="68">M16-M18</f>
+        <f t="shared" ref="M20:Q20" si="68">M16-M18</f>
         <v>4.21381206490129E-4</v>
       </c>
       <c r="N20" s="3">
@@ -29554,7 +29550,7 @@
       <c r="J25" s="1"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3">
-        <f t="shared" ref="L25:Q25" si="88">M23-M22</f>
+        <f t="shared" ref="M25:Q25" si="88">M23-M22</f>
         <v>3.5822061403076311E-4</v>
       </c>
       <c r="N25" s="3">
@@ -29617,7 +29613,7 @@
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="3">
-        <f t="shared" ref="L26:Q26" si="91">M22-M24</f>
+        <f t="shared" ref="M26:Q26" si="91">M22-M24</f>
         <v>3.5661202493345034E-4</v>
       </c>
       <c r="N26" s="3">
@@ -29808,7 +29804,7 @@
       <c r="J31" s="1"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3">
-        <f t="shared" ref="L31:Q31" si="111">M29-M28</f>
+        <f t="shared" ref="M31:Q31" si="111">M29-M28</f>
         <v>3.8081897933431308E-4</v>
       </c>
       <c r="N31" s="3">
@@ -29871,7 +29867,7 @@
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="3">
-        <f t="shared" ref="L32:Q32" si="114">M28-M30</f>
+        <f t="shared" ref="M32:Q32" si="114">M28-M30</f>
         <v>3.790052746989736E-4</v>
       </c>
       <c r="N32" s="3">
@@ -29906,6 +29902,9 @@
       <c r="C34">
         <v>17.510000000000002</v>
       </c>
+      <c r="D34" s="13">
+        <v>17.510000000000002</v>
+      </c>
       <c r="L34" s="3">
         <f>1/C34</f>
         <v>5.711022272986864E-2</v>
@@ -29916,6 +29915,9 @@
         <v>0</v>
       </c>
       <c r="C35">
+        <v>0.27</v>
+      </c>
+      <c r="D35" s="13">
         <v>0.27</v>
       </c>
       <c r="L35" s="4">
@@ -29929,7 +29931,7 @@
         <v>5.6242969628796394E-2</v>
       </c>
       <c r="V36">
-        <f t="shared" ref="V36:AB36" si="116">M2</f>
+        <f t="shared" ref="V36:Z36" si="116">M2</f>
         <v>0.125</v>
       </c>
       <c r="W36">
@@ -30042,9 +30044,11 @@
         <v>20.893605734201135</v>
       </c>
       <c r="AM38">
+        <f>$C$34</f>
         <v>17.510000000000002</v>
       </c>
       <c r="AN38">
+        <f>$C$35</f>
         <v>0.27</v>
       </c>
       <c r="AO38" s="2">
@@ -30115,9 +30119,11 @@
         <v>15.820284680275169</v>
       </c>
       <c r="AM41">
+        <f t="shared" ref="AM39:AM50" si="117">$C$34</f>
         <v>17.510000000000002</v>
       </c>
       <c r="AN41">
+        <f t="shared" ref="AN39:AN50" si="118">$C$35</f>
         <v>0.27</v>
       </c>
       <c r="AO41" s="2">
@@ -30188,9 +30194,11 @@
         <v>12.657616823133935</v>
       </c>
       <c r="AM44">
+        <f t="shared" si="117"/>
         <v>17.510000000000002</v>
       </c>
       <c r="AN44">
+        <f t="shared" si="118"/>
         <v>0.27</v>
       </c>
       <c r="AO44" s="2">
@@ -30261,9 +30269,11 @@
         <v>12.092699531627739</v>
       </c>
       <c r="AM47">
+        <f t="shared" si="117"/>
         <v>17.510000000000002</v>
       </c>
       <c r="AN47">
+        <f t="shared" si="118"/>
         <v>0.27</v>
       </c>
       <c r="AO47" s="2">
@@ -30334,9 +30344,11 @@
         <v>12.359932517346573</v>
       </c>
       <c r="AM50">
+        <f t="shared" si="117"/>
         <v>17.510000000000002</v>
       </c>
       <c r="AN50">
+        <f t="shared" si="118"/>
         <v>0.27</v>
       </c>
       <c r="AO50" s="2">

</xml_diff>